<commit_message>
0.2 noozle miniatures profile added
</commit_message>
<xml_diff>
--- a/Valor_Impressao_3D.xlsx
+++ b/Valor_Impressao_3D.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Google Drive/3D/3D_printing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4D46CF-D2F5-0546-BAD6-74545DEC9813}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D970DAB-0D3A-854C-92B1-1F0597B1E5F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1251,7 +1251,7 @@
   <dimension ref="B3:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1289,7 +1289,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>41</v>
@@ -1298,7 +1298,7 @@
     <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="40"/>
       <c r="C7" s="14">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>10</v>
@@ -1309,7 +1309,7 @@
         <v>50</v>
       </c>
       <c r="C8" s="16">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>7</v>
@@ -1484,7 +1484,7 @@
         <v>48</v>
       </c>
       <c r="C25" s="23">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>19</v>
@@ -1555,7 +1555,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="8">
         <f>SUM(C42:C47)+C49+C50</f>
-        <v>9.8831496000000012</v>
+        <v>4.4423482906666667</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1565,7 +1565,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="10">
         <f>D32*(1+C30/100)</f>
-        <v>14.824724400000001</v>
+        <v>6.663522436</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1575,7 +1575,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="10">
         <f>D33*(1+C29/100)</f>
-        <v>14.824724400000001</v>
+        <v>6.663522436</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1585,7 +1585,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="10">
         <f>D33*(1+C28/100)+C27</f>
-        <v>21.455444084000003</v>
+        <v>12.396509903960002</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1595,7 +1595,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="10">
         <f>D34*(1+C28/100)+C27</f>
-        <v>21.455444084000003</v>
+        <v>12.396509903960002</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1605,7 +1605,7 @@
       <c r="C37" s="7"/>
       <c r="D37" s="11">
         <f>D33*C9</f>
-        <v>14.824724400000001</v>
+        <v>6.663522436</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1615,7 +1615,7 @@
       <c r="C38" s="7"/>
       <c r="D38" s="11">
         <f>D34*C9</f>
-        <v>14.824724400000001</v>
+        <v>6.663522436</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1625,7 +1625,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="11">
         <f>D37*(1+C28/100)+C27</f>
-        <v>21.455444084000003</v>
+        <v>12.396509903960002</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1635,7 +1635,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="10">
         <f>D38*(1+C28/100)+C27</f>
-        <v>21.455444084000003</v>
+        <v>12.396509903960002</v>
       </c>
     </row>
     <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="C42" s="4">
         <f>(C11/1000)*C8</f>
-        <v>2.2000000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>18</v>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C43" s="4">
         <f>C14/1000*C20*(C6+C7/60)</f>
-        <v>0.85407480000000002</v>
+        <v>0.74494302000000001</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>18</v>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C45" s="4">
         <f>(C42+C43+C44)*C25/100</f>
-        <v>3.5540748000000004</v>
+        <v>0.33698860400000002</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>18</v>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="C46" s="4">
         <f>C21/6000*(C6+C7/60)</f>
-        <v>0.89999999999999991</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>18</v>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="C49" s="32">
         <f>(C21/(C24*C23*C22))*(C6+C7/60)</f>
-        <v>1.875</v>
+        <v>1.6354166666666667</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
planilha de custos atualizada
</commit_message>
<xml_diff>
--- a/Valor_Impressao_3D.xlsx
+++ b/Valor_Impressao_3D.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Google Drive/3D/3D_printing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D970DAB-0D3A-854C-92B1-1F0597B1E5F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84CED1B-5811-1040-A9BA-702EEE73C9D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,10 @@
     <author>claudio jesus russo</author>
     <author>Jasmine Moreira</author>
     <author>Russo Claudio (LBR)</author>
+    <author>.</author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="1" shapeId="0" xr:uid="{650D9A70-EDC2-A34C-B2B9-E9CB43614281}">
+    <comment ref="B11" authorId="1" shapeId="0" xr:uid="{650D9A70-EDC2-A34C-B2B9-E9CB43614281}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="1" shapeId="0" xr:uid="{9092EF8A-2ED9-574E-A7B3-B67823106802}">
+    <comment ref="B12" authorId="1" shapeId="0" xr:uid="{9092EF8A-2ED9-574E-A7B3-B67823106802}">
       <text>
         <r>
           <rPr>
@@ -119,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -133,21 +134,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="1" shapeId="0" xr:uid="{0CA1516E-75EF-5841-8B9B-7E887AEDF6B1}">
+    <comment ref="B15" authorId="3" shapeId="0" xr:uid="{D095B44D-431B-AB48-ADD5-746AC9309553}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Custo individual
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Modelagem, envio, embalagem, comissão, taxas extras...</t>
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B17" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +181,49 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B20" authorId="3" shapeId="0" xr:uid="{8A23A2BE-9A88-994E-A43C-2777755B5C90}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">aproximadamente:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">8h x 5d x 52sem x 3anos
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="1" shapeId="0" xr:uid="{54A64829-89B6-A641-9A0F-5C5FD1723EAA}">
+    <comment ref="B37" authorId="1" shapeId="0" xr:uid="{54A64829-89B6-A641-9A0F-5C5FD1723EAA}">
       <text>
         <r>
           <rPr>
@@ -208,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="1" shapeId="0" xr:uid="{903388DA-A8BE-1843-9046-D4FF10AD0FF8}">
+    <comment ref="B38" authorId="1" shapeId="0" xr:uid="{903388DA-A8BE-1843-9046-D4FF10AD0FF8}">
       <text>
         <r>
           <rPr>
@@ -241,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B50" authorId="1" shapeId="0" xr:uid="{FBD6FD35-9A80-5940-8637-D94AFCAC6E61}">
+    <comment ref="B42" authorId="1" shapeId="0" xr:uid="{FBD6FD35-9A80-5940-8637-D94AFCAC6E61}">
       <text>
         <r>
           <rPr>
@@ -279,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Retorno de investimento</t>
   </si>
@@ -308,9 +370,6 @@
     <t>RESULTADO</t>
   </si>
   <si>
-    <t>Modelagem 3D</t>
-  </si>
-  <si>
     <t>min</t>
   </si>
   <si>
@@ -326,9 +385,6 @@
     <t>Outros custos</t>
   </si>
   <si>
-    <t>jasmine.moreira.2013@gmail.com</t>
-  </si>
-  <si>
     <t>Imposto</t>
   </si>
   <si>
@@ -359,12 +415,6 @@
     <t>Taxas</t>
   </si>
   <si>
-    <t>Taxa de anúncio ML</t>
-  </si>
-  <si>
-    <t>Taxa de venda ML</t>
-  </si>
-  <si>
     <t>Taxa de lucro</t>
   </si>
   <si>
@@ -383,12 +433,6 @@
     <t>Unidade com Imposto</t>
   </si>
   <si>
-    <t>Unidade ML sem Imposto</t>
-  </si>
-  <si>
-    <t>Unidade ML com Imposto</t>
-  </si>
-  <si>
     <t>Unidade sem Imposto</t>
   </si>
   <si>
@@ -398,18 +442,9 @@
     <t>Lote com Imposto</t>
   </si>
   <si>
-    <t>Lote ML sem Imposto</t>
-  </si>
-  <si>
-    <t>Lote ML com Imposto</t>
-  </si>
-  <si>
     <t>h</t>
   </si>
   <si>
-    <t>VALOR DA IMPRESSÃO 3D - V1.1</t>
-  </si>
-  <si>
     <t>Parâmetros da Máquina</t>
   </si>
   <si>
@@ -440,13 +475,16 @@
     <t>Custo  de acabamento por unidade</t>
   </si>
   <si>
-    <t>Custo de postagem por unidade</t>
-  </si>
-  <si>
-    <t>Custo de embalagem por unidade</t>
-  </si>
-  <si>
     <t>Valor de produção por unidade</t>
+  </si>
+  <si>
+    <t>Cultura Maker</t>
+  </si>
+  <si>
+    <t>Tempo de depreciação</t>
+  </si>
+  <si>
+    <t>VALOR DA IMPRESSÃO 3D - V1.2</t>
   </si>
 </sst>
 </file>
@@ -458,7 +496,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +636,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="14">
@@ -773,7 +816,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -787,9 +830,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -859,12 +899,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -894,6 +928,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1248,525 +1285,451 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D50"/>
+  <dimension ref="B2:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="31"/>
-    <col min="2" max="2" width="29.1640625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="31" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="31"/>
+    <col min="1" max="1" width="23" style="28" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="28" customWidth="1"/>
+    <col min="5" max="7" width="9.1640625" style="28"/>
+    <col min="8" max="8" width="9.1640625" style="28" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="28"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+    </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+    </row>
+    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+    </row>
+    <row r="5" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="11">
+        <v>15</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="37"/>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="15">
+        <v>39</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="19">
+        <v>10</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+    </row>
+    <row r="10" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="21">
+        <v>110</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
+      <c r="C11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="21">
+        <v>0.79081000000000001</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+    </row>
+    <row r="15" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21">
+        <v>0</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+    </row>
+    <row r="17" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="22">
+        <v>360</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="24">
+        <v>1800</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="25">
+        <v>36</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="25">
+        <v>6000</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="27">
+        <v>10</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="25">
+        <v>8</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="22">
+        <v>20</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+    </row>
+    <row r="25" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="22">
+        <v>10</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="22">
+        <v>50</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7">
+        <f>SUM(C34:C39)+C41+C42</f>
+        <v>25.747448800000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="B29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="9">
+        <f>D28*(1+C26/100)</f>
+        <v>38.621173200000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="B30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-    </row>
-    <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="C30" s="6"/>
+      <c r="D30" s="9">
+        <f>D29*(1+C25/100)</f>
+        <v>42.483290520000004</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="B31" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="10">
+        <f>D29*C8</f>
+        <v>386.21173199999998</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="B32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="10">
+        <f>D30*C8</f>
+        <v>424.83290520000003</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+    </row>
+    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="4">
+        <f>(C10/1000)*C7</f>
+        <v>4.29</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4">
+        <f>C13/1000*C17*(C5+C6/60)</f>
+        <v>4.2703739999999994</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="4">
+        <f>C11</f>
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="40"/>
-      <c r="C7" s="14">
-        <v>37</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="16">
-        <v>4</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="20">
+      <c r="C37" s="4">
+        <f>(C34+C35+C36)*C23/100</f>
+        <v>1.8120747999999998</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="4">
+        <f>C18/C20*(C5+C6/60)</f>
+        <v>4.5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="4">
+        <f>C12</f>
         <v>1</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="22">
-        <v>110</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="19">
+      <c r="D39" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+    </row>
+    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="22">
-        <v>0.79081000000000001</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="22">
+      <c r="C41" s="29">
+        <f>(C18/(C22*C21*C19))*(C5+C6/60)</f>
+        <v>9.375</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="38">
+        <f>C15</f>
         <v>0</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="22">
-        <v>0</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="22">
-        <v>0</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="23">
-        <v>360</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="25">
-        <v>1800</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="26">
-        <v>36</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="28">
-        <v>10</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="26">
-        <v>8</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="23">
-        <v>20</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="22">
-        <v>5</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="23">
-        <v>11</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
+      <c r="D42" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C29" s="23">
-        <v>0</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="23">
-        <v>50</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-    </row>
-    <row r="32" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8">
-        <f>SUM(C42:C47)+C49+C50</f>
-        <v>4.4423482906666667</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B33" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="10">
-        <f>D32*(1+C30/100)</f>
-        <v>6.663522436</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B34" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="10">
-        <f>D33*(1+C29/100)</f>
-        <v>6.663522436</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B35" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="10">
-        <f>D33*(1+C28/100)+C27</f>
-        <v>12.396509903960002</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B36" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="10">
-        <f>D34*(1+C28/100)+C27</f>
-        <v>12.396509903960002</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B37" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="11">
-        <f>D33*C9</f>
-        <v>6.663522436</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B38" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="11">
-        <f>D34*C9</f>
-        <v>6.663522436</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B39" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="11">
-        <f>D37*(1+C28/100)+C27</f>
-        <v>12.396509903960002</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B40" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="10">
-        <f>D38*(1+C28/100)+C27</f>
-        <v>12.396509903960002</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-    </row>
-    <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="4">
-        <f>(C11/1000)*C8</f>
-        <v>0.44</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="4">
-        <f>C14/1000*C20*(C6+C7/60)</f>
-        <v>0.74494302000000001</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="4">
-        <f>C12</f>
-        <v>0.5</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="4">
-        <f>(C42+C43+C44)*C25/100</f>
-        <v>0.33698860400000002</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="4">
-        <f>C21/6000*(C6+C7/60)</f>
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="4">
-        <f>C13</f>
-        <v>0</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-    </row>
-    <row r="49" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="32">
-        <f>(C21/(C24*C23*C22))*(C6+C7/60)</f>
-        <v>1.6354166666666667</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="5">
-        <f>C16/C9+C17+C18</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{FF285AC1-EBD2-AC43-8AF6-07C834979D4F}"/>
-  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
novos perfis médios para ABS e PLA
</commit_message>
<xml_diff>
--- a/Valor_Impressao_3D.xlsx
+++ b/Valor_Impressao_3D.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Google Drive/3D/3D_printing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84CED1B-5811-1040-A9BA-702EEE73C9D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC80D4F4-5ACC-3841-8126-C80FD7A7C447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,6 +905,9 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,9 +931,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1288,7 +1288,7 @@
   <dimension ref="B2:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1303,39 +1303,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="11">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="13">
         <v>0</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>41</v>
       </c>
       <c r="C7" s="15">
-        <v>39</v>
+        <v>200</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>7</v>
@@ -1359,53 +1359,53 @@
         <v>26</v>
       </c>
       <c r="C8" s="19">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-    </row>
-    <row r="10" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="21">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="21">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="18">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
         <v>6</v>
       </c>
@@ -1416,14 +1416,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="34" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-    </row>
-    <row r="15" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
         <v>1</v>
       </c>
@@ -1434,14 +1434,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:4" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="34" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-    </row>
-    <row r="17" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+    </row>
+    <row r="17" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="s">
         <v>28</v>
       </c>
@@ -1452,18 +1452,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="24">
-        <v>1800</v>
+        <v>2500</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
         <v>36</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B20" s="23" t="s">
         <v>46</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B21" s="23" t="s">
         <v>37</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
         <v>38</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="s">
         <v>39</v>
       </c>
@@ -1518,25 +1518,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:4" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="34" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-    </row>
-    <row r="25" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+    </row>
+    <row r="25" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="22">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D25" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B26" s="20" t="s">
         <v>24</v>
       </c>
@@ -1547,12 +1547,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="15" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="35" t="s">
+    <row r="27" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
     </row>
     <row r="28" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
@@ -1561,7 +1561,7 @@
       <c r="C28" s="6"/>
       <c r="D28" s="7">
         <f>SUM(C34:C39)+C41+C42</f>
-        <v>25.747448800000001</v>
+        <v>173.85408568888892</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1571,7 +1571,7 @@
       <c r="C29" s="6"/>
       <c r="D29" s="9">
         <f>D28*(1+C26/100)</f>
-        <v>38.621173200000001</v>
+        <v>260.78112853333334</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1581,7 +1581,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="9">
         <f>D29*(1+C25/100)</f>
-        <v>42.483290520000004</v>
+        <v>260.78112853333334</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1591,7 +1591,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="10">
         <f>D29*C8</f>
-        <v>386.21173199999998</v>
+        <v>260.78112853333334</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="19" x14ac:dyDescent="0.2">
@@ -1601,15 +1601,15 @@
       <c r="C32" s="6"/>
       <c r="D32" s="10">
         <f>D30*C8</f>
-        <v>424.83290520000003</v>
+        <v>260.78112853333334</v>
       </c>
     </row>
     <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
     </row>
     <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="C34" s="4">
         <f>(C10/1000)*C7</f>
-        <v>4.29</v>
+        <v>24</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>16</v>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="C35" s="4">
         <f>C13/1000*C17*(C5+C6/60)</f>
-        <v>4.2703739999999994</v>
+        <v>11.387663999999999</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>16</v>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="C36" s="4">
         <f>C11</f>
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>16</v>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="C37" s="4">
         <f>(C34+C35+C36)*C23/100</f>
-        <v>1.8120747999999998</v>
+        <v>17.0775328</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>16</v>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="C38" s="4">
         <f>C18/C20*(C5+C6/60)</f>
-        <v>4.5</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>16</v>
@@ -1677,18 +1677,18 @@
       </c>
       <c r="C39" s="4">
         <f>C12</f>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
     </row>
     <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="C41" s="29">
         <f>(C18/(C22*C21*C19))*(C5+C6/60)</f>
-        <v>9.375</v>
+        <v>34.722222222222221</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>16</v>
@@ -1706,7 +1706,7 @@
       <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="38">
+      <c r="C42" s="30">
         <f>C15</f>
         <v>0</v>
       </c>

</xml_diff>